<commit_message>
Crea fichero elementos completo
</commit_message>
<xml_diff>
--- a/AutomatizaElementos/CT102A_datosEspecificos.xlsx
+++ b/AutomatizaElementos/CT102A_datosEspecificos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>key</t>
   </si>
@@ -92,6 +92,30 @@
   </si>
   <si>
     <t>ESP-postalCodeDirector</t>
+  </si>
+  <si>
+    <t>CODIGO_DELEGACION</t>
+  </si>
+  <si>
+    <t>IDIOMA_EXPEDIENTE</t>
+  </si>
+  <si>
+    <t>MEDIO_NOTIFICACION</t>
+  </si>
+  <si>
+    <t>INTERESADO_NOTIFICACION</t>
+  </si>
+  <si>
+    <t>//ProcedimientoXunta/SI460A_4/Delegacion/cmbDelegacion</t>
+  </si>
+  <si>
+    <t>//ProcedimientoXunta/SI460A_4/Delegacion/txtIdioma</t>
+  </si>
+  <si>
+    <t>//ProcedimientoXunta/SI460A/Notificacion/rblModalidad</t>
+  </si>
+  <si>
+    <t>//ProcedimientoXunta/SI460A/Notificacion/rbNotificar</t>
   </si>
 </sst>
 </file>
@@ -444,15 +468,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
@@ -482,81 +506,113 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F9" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Distingue entre RB, Checks y campos de texto + formateoXML
</commit_message>
<xml_diff>
--- a/AutomatizaElementos/CT102A_datosEspecificos.xlsx
+++ b/AutomatizaElementos/CT102A_datosEspecificos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>key</t>
   </si>
@@ -46,9 +46,6 @@
     <t>String</t>
   </si>
   <si>
-    <t>//ProcedimientoXunta/CT102A/Director/txtNombre</t>
-  </si>
-  <si>
     <t>ESP-directorName</t>
   </si>
   <si>
@@ -76,15 +73,6 @@
     <t>CP director</t>
   </si>
   <si>
-    <t>//ProcedimientoXunta/CT102A/Director/txtApel1</t>
-  </si>
-  <si>
-    <t>//ProcedimientoXunta/CT102A/Director/txtApel2</t>
-  </si>
-  <si>
-    <t>//ProcedimientoXunta/CT102A/Director/txtCp</t>
-  </si>
-  <si>
     <t>ESP-lastName2</t>
   </si>
   <si>
@@ -106,16 +94,58 @@
     <t>INTERESADO_NOTIFICACION</t>
   </si>
   <si>
-    <t>//ProcedimientoXunta/SI460A_4/Delegacion/cmbDelegacion</t>
-  </si>
-  <si>
-    <t>//ProcedimientoXunta/SI460A_4/Delegacion/txtIdioma</t>
-  </si>
-  <si>
-    <t>//ProcedimientoXunta/SI460A/Notificacion/rblModalidad</t>
-  </si>
-  <si>
-    <t>//ProcedimientoXunta/SI460A/Notificacion/rbNotificar</t>
+    <t>/ProcedimientoXunta/SI460A_4/Delegacion/cmbDelegacion</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/SI460A_4/Delegacion/txtIdioma</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/SI460A/Notificacion/rblModalidad</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/SI460A/Notificacion/rbNotificar</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/CT102A/Director/txtNombre</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/CT102A/Director/txtApel1</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/CT102A/Director/txtApel2</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/CT102A/Director/txtCp</t>
+  </si>
+  <si>
+    <t>sexoDirector</t>
+  </si>
+  <si>
+    <t>Sexo director</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/CT102A/Director/rbSexo</t>
+  </si>
+  <si>
+    <t>ESP-sexDirector</t>
+  </si>
+  <si>
+    <t>sabeIngles</t>
+  </si>
+  <si>
+    <t>Sabe inglés</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/CT102A/Director/chSabe</t>
+  </si>
+  <si>
+    <t>ESP-englishKnowledge</t>
   </si>
 </sst>
 </file>
@@ -468,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,34 +536,34 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
         <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
         <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -550,70 +580,110 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
         <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Genera campos de comprobación de Datos
</commit_message>
<xml_diff>
--- a/AutomatizaElementos/CT102A_datosEspecificos.xlsx
+++ b/AutomatizaElementos/CT102A_datosEspecificos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>key</t>
   </si>
@@ -146,6 +146,39 @@
   </si>
   <si>
     <t>ESP-englishKnowledge</t>
+  </si>
+  <si>
+    <t>estrella</t>
+  </si>
+  <si>
+    <t>autSviRep</t>
+  </si>
+  <si>
+    <t>Autorización SVI representante</t>
+  </si>
+  <si>
+    <t>DEN_SVI_REP</t>
+  </si>
+  <si>
+    <t>DENSVI_REPRES</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/SI452A_2/ComprobacionDatos/tblDatos/FilaA2/cvDeniego</t>
+  </si>
+  <si>
+    <t>autSviSol</t>
+  </si>
+  <si>
+    <t>Autorización SVI solicitante</t>
+  </si>
+  <si>
+    <t>DENSVI_PRESENT</t>
+  </si>
+  <si>
+    <t>DEN_SVI_SOL</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -498,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,11 +543,12 @@
     <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="83.5703125" customWidth="1"/>
+    <col min="5" max="5" width="59" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,40 +567,55 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -585,8 +634,11 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -605,8 +657,11 @@
       <c r="F7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -625,8 +680,11 @@
       <c r="F8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -645,8 +703,11 @@
       <c r="F9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -665,8 +726,11 @@
       <c r="F10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -684,6 +748,55 @@
       </c>
       <c r="F11" t="s">
         <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejora en el formateo de XML
</commit_message>
<xml_diff>
--- a/AutomatizaElementos/CT102A_datosEspecificos.xlsx
+++ b/AutomatizaElementos/CT102A_datosEspecificos.xlsx
@@ -136,49 +136,49 @@
     <t>sabeIngles</t>
   </si>
   <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/CT102A/Director/chSabe</t>
+  </si>
+  <si>
+    <t>ESP-englishKnowledge</t>
+  </si>
+  <si>
+    <t>estrella</t>
+  </si>
+  <si>
+    <t>autSviRep</t>
+  </si>
+  <si>
+    <t>DEN_SVI_REP</t>
+  </si>
+  <si>
+    <t>DENSVI_REPRES</t>
+  </si>
+  <si>
+    <t>/ProcedimientoXunta/SI452A_2/ComprobacionDatos/tblDatos/FilaA2/cvDeniego</t>
+  </si>
+  <si>
+    <t>autSviSol</t>
+  </si>
+  <si>
+    <t>DENSVI_PRESENT</t>
+  </si>
+  <si>
+    <t>DEN_SVI_SOL</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>Sabe inglés</t>
   </si>
   <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>/ProcedimientoXunta/CT102A/Director/chSabe</t>
-  </si>
-  <si>
-    <t>ESP-englishKnowledge</t>
-  </si>
-  <si>
-    <t>estrella</t>
-  </si>
-  <si>
-    <t>autSviRep</t>
-  </si>
-  <si>
     <t>Autorización SVI representante</t>
   </si>
   <si>
-    <t>DEN_SVI_REP</t>
-  </si>
-  <si>
-    <t>DENSVI_REPRES</t>
-  </si>
-  <si>
-    <t>/ProcedimientoXunta/SI452A_2/ComprobacionDatos/tblDatos/FilaA2/cvDeniego</t>
-  </si>
-  <si>
-    <t>autSviSol</t>
-  </si>
-  <si>
     <t>Autorización SVI solicitante</t>
-  </si>
-  <si>
-    <t>DENSVI_PRESENT</t>
-  </si>
-  <si>
-    <t>DEN_SVI_SOL</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +568,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -590,7 +590,7 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
         <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -658,7 +658,7 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -704,7 +704,7 @@
         <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -735,68 +735,68 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
         <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" t="s">
         <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>